<commit_message>
add env & fix file upload error
</commit_message>
<xml_diff>
--- a/Filled_GLA_AEB_start_forms_.xlsx
+++ b/Filled_GLA_AEB_start_forms_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Prevista\GLA-form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9991AA95-CA3D-41E5-B391-CC47EBEFD523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17887522-6A8F-4FE6-AEE5-278BD90191F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ILR" sheetId="16" r:id="rId1"/>
@@ -6425,7 +6425,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1925B180-D33C-FB32-2388-6D626AD04395}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C2B7C52-C803-E13D-5035-D0402911A668}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7158,7 +7158,7 @@
         <xdr:cNvPr id="16" name="Picture 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59C04EEE-A44B-2D5F-14F8-001FB69F9641}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CE9F6EB-2129-762D-BCB0-E04DDC07EBBF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18022,7 +18022,7 @@
       <c r="V37" s="384"/>
       <c r="W37" s="384"/>
       <c r="X37" s="390" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="Y37" s="390"/>
       <c r="Z37" s="390"/>
@@ -18296,7 +18296,7 @@
       <c r="AK42" s="405"/>
       <c r="AL42" s="405"/>
       <c r="AM42" s="406" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="AN42" s="452"/>
       <c r="AO42" s="3"/>
@@ -18497,7 +18497,7 @@
       <c r="AJ46" s="456"/>
       <c r="AK46" s="457"/>
       <c r="AL46" s="453" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="AM46" s="453"/>
       <c r="AN46" s="454"/>

</xml_diff>